<commit_message>
UploadCountryVersion Tested and Working
</commit_message>
<xml_diff>
--- a/MethodsToDo.xlsx
+++ b/MethodsToDo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dhaen\EindwerkPG1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{12DF5E1A-5CE2-4C46-85BA-BCE51CF44902}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{524B65DF-A8A8-4FF7-9420-F205F8B79FD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{1ED8FFE9-2422-4037-B33C-0042EE26BDD6}"/>
   </bookViews>
@@ -517,7 +517,7 @@
   <dimension ref="A2:B39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -555,8 +555,8 @@
       <c r="A9" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>8</v>
+      <c r="B9" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
All Repositories Upload methods tested and working
</commit_message>
<xml_diff>
--- a/MethodsToDo.xlsx
+++ b/MethodsToDo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dhaen\EindwerkPG1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{524B65DF-A8A8-4FF7-9420-F205F8B79FD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47FDC816-B76D-4EE4-A1BF-0CE51D04C318}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{1ED8FFE9-2422-4037-B33C-0042EE26BDD6}"/>
   </bookViews>
@@ -516,8 +516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D3E43DF-7AED-46EF-8568-98DFF9071DBA}">
   <dimension ref="A2:B39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -534,8 +534,8 @@
       <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>8</v>
+      <c r="B4" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -568,8 +568,8 @@
       <c r="A13" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>8</v>
+      <c r="B13" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -589,8 +589,8 @@
       <c r="A18" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>8</v>
+      <c r="B18" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -610,16 +610,16 @@
       <c r="A23" t="s">
         <v>14</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>8</v>
+      <c r="B23" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>15</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>8</v>
+      <c r="B24" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
@@ -647,24 +647,24 @@
       <c r="A30" t="s">
         <v>19</v>
       </c>
-      <c r="B30" s="3" t="s">
-        <v>8</v>
+      <c r="B30" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>20</v>
       </c>
-      <c r="B31" s="3" t="s">
-        <v>8</v>
+      <c r="B31" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>21</v>
       </c>
-      <c r="B32" s="3" t="s">
-        <v>8</v>
+      <c r="B32" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
DatabaseReaders Simulation Done + Tested
</commit_message>
<xml_diff>
--- a/MethodsToDo.xlsx
+++ b/MethodsToDo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dhaen\EindwerkPG1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47FDC816-B76D-4EE4-A1BF-0CE51D04C318}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83BD9CAB-E7FD-4E59-A3E3-219BC026A84F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{1ED8FFE9-2422-4037-B33C-0042EE26BDD6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="27">
   <si>
     <t>AddressRepository</t>
   </si>
@@ -44,9 +44,6 @@
     <t>UploadAddress</t>
   </si>
   <si>
-    <t>GetAddressByCountryID</t>
-  </si>
-  <si>
     <t>DONE</t>
   </si>
   <si>
@@ -62,9 +59,6 @@
     <t>UploadCustomer</t>
   </si>
   <si>
-    <t>TODO</t>
-  </si>
-  <si>
     <t>GetCustomerBySimulationID</t>
   </si>
   <si>
@@ -74,9 +68,6 @@
     <t>UploadMunicipality</t>
   </si>
   <si>
-    <t>GetMunicipalityByCountryID</t>
-  </si>
-  <si>
     <t>NameRepository</t>
   </si>
   <si>
@@ -86,12 +77,6 @@
     <t>UploadLastName</t>
   </si>
   <si>
-    <t>GetFirstNameByCountryID</t>
-  </si>
-  <si>
-    <t>GetLastNameByCountryID</t>
-  </si>
-  <si>
     <t>SimulationRepository</t>
   </si>
   <si>
@@ -107,12 +92,6 @@
     <t>GetSimulationDataByID</t>
   </si>
   <si>
-    <t>GetSimulationSettingsBySImulationID</t>
-  </si>
-  <si>
-    <t>GetSimulationStatisticsBySimulationID</t>
-  </si>
-  <si>
     <t>CsvFileReader</t>
   </si>
   <si>
@@ -120,6 +99,24 @@
   </si>
   <si>
     <t>JSonFileReader</t>
+  </si>
+  <si>
+    <t>GetAddressByCountryVersionID</t>
+  </si>
+  <si>
+    <t>GetSimulationSettingsBySImulationDataID</t>
+  </si>
+  <si>
+    <t>GetSimulationStatisticsBySimulationDataID</t>
+  </si>
+  <si>
+    <t>GetMunicipalityByCountryVersionID</t>
+  </si>
+  <si>
+    <t>GetFirstNameByCountryVersionID</t>
+  </si>
+  <si>
+    <t>GetLastNameByCountryVersionID</t>
   </si>
 </sst>
 </file>
@@ -143,7 +140,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -153,12 +150,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -175,11 +166,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -516,13 +506,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D3E43DF-7AED-46EF-8568-98DFF9071DBA}">
   <dimension ref="A2:B39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -535,184 +525,184 @@
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>8</v>
+        <v>21</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>12</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>8</v>
+        <v>24</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>16</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>8</v>
+        <v>25</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>17</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>8</v>
+        <v>26</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>22</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>23</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>24</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>8</v>
+        <v>23</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>